<commit_message>
Dodawanie nowych rodzajów ziaren poprzez kliknięcie myszką
</commit_message>
<xml_diff>
--- a/Postępy prac.xlsx
+++ b/Postępy prac.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
@@ -204,7 +204,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -212,9 +212,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -252,7 +252,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -322,7 +322,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -499,7 +499,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -557,19 +557,19 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="1"/>
@@ -578,19 +578,19 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="1"/>

</xml_diff>

<commit_message>
Dodanie mpi.jar bezpośrednio do projektu. Dodania pliku uruchomieniowego ziarna.jar
</commit_message>
<xml_diff>
--- a/Postępy prac.xlsx
+++ b/Postępy prac.xlsx
@@ -125,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,12 +141,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -190,9 +184,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -492,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -542,7 +533,7 @@
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1"/>
@@ -551,19 +542,19 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="1"/>
@@ -572,7 +563,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -593,19 +584,19 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="1"/>
@@ -614,19 +605,19 @@
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="1"/>
@@ -635,19 +626,19 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="1"/>

</xml_diff>